<commit_message>
Building Effective Data Tables in Excel
</commit_message>
<xml_diff>
--- a/Section 29: Mastering Excel's "What If?" Tools/Resources/Excel103-AdvancedExercises.xlsx
+++ b/Section 29: Mastering Excel's "What If?" Tools/Resources/Excel103-AdvancedExercises.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11116"/>
   <workbookPr codeName="ThisWorkbook" checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolinecrandell/Documents/Employment/*Applications/2022.12 Job Apps/GitHub/excel/Section 29: Mastering Excel's &quot;What If?&quot; Tools/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E550A1-0349-A147-903C-7262AB0CF9DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548E3918-08AE-FA4C-AC94-FFE5248D8570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16680" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16680" firstSheet="7" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -1972,13 +1972,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3046,10 +3046,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="134" t="s">
+      <c r="E2" s="136" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="134"/>
+      <c r="F2" s="136"/>
     </row>
     <row r="3" spans="2:6" ht="14">
       <c r="B3" s="25" t="s">
@@ -3058,11 +3058,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="135" t="str">
+      <c r="E3" s="134" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="136"/>
+      <c r="F3" s="135"/>
     </row>
     <row r="4" spans="2:6" ht="14">
       <c r="B4" s="25" t="s">
@@ -3071,11 +3071,11 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="135" t="str">
+      <c r="E4" s="134" t="str">
         <f>_xlfn.CONCAT(C4, " ", B4)</f>
         <v>Joe Gonzales</v>
       </c>
-      <c r="F4" s="136"/>
+      <c r="F4" s="135"/>
     </row>
     <row r="5" spans="2:6" ht="14">
       <c r="B5" s="25" t="s">
@@ -3084,11 +3084,11 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="135" t="str">
+      <c r="E5" s="134" t="str">
         <f t="shared" ref="E5:E17" si="0">_xlfn.CONCAT(C5, " ", B5)</f>
         <v>Gail Scote</v>
       </c>
-      <c r="F5" s="136"/>
+      <c r="F5" s="135"/>
     </row>
     <row r="6" spans="2:6" ht="14">
       <c r="B6" s="25" t="s">
@@ -3097,11 +3097,11 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="135" t="str">
+      <c r="E6" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Sheryl Kane</v>
       </c>
-      <c r="F6" s="136"/>
+      <c r="F6" s="135"/>
     </row>
     <row r="7" spans="2:6" ht="14">
       <c r="B7" s="25" t="s">
@@ -3110,11 +3110,11 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="135" t="str">
+      <c r="E7" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Kendrick Hapsbuch</v>
       </c>
-      <c r="F7" s="136"/>
+      <c r="F7" s="135"/>
     </row>
     <row r="8" spans="2:6" ht="14">
       <c r="B8" s="25" t="s">
@@ -3123,11 +3123,11 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="135" t="str">
+      <c r="E8" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Mark Henders</v>
       </c>
-      <c r="F8" s="136"/>
+      <c r="F8" s="135"/>
     </row>
     <row r="9" spans="2:6" ht="14">
       <c r="B9" s="25" t="s">
@@ -3136,11 +3136,11 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="135" t="str">
+      <c r="E9" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Katie Atherton</v>
       </c>
-      <c r="F9" s="136"/>
+      <c r="F9" s="135"/>
     </row>
     <row r="10" spans="2:6" ht="14">
       <c r="B10" s="25" t="s">
@@ -3149,11 +3149,11 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="135" t="str">
+      <c r="E10" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Frank Bellwood</v>
       </c>
-      <c r="F10" s="136"/>
+      <c r="F10" s="135"/>
     </row>
     <row r="11" spans="2:6" ht="14">
       <c r="B11" s="25" t="s">
@@ -3162,11 +3162,11 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="135" t="str">
+      <c r="E11" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Linda Cooper</v>
       </c>
-      <c r="F11" s="136"/>
+      <c r="F11" s="135"/>
     </row>
     <row r="12" spans="2:6" ht="14">
       <c r="B12" s="25" t="s">
@@ -3175,11 +3175,11 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="135" t="str">
+      <c r="E12" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Brent Cronwith</v>
       </c>
-      <c r="F12" s="136"/>
+      <c r="F12" s="135"/>
     </row>
     <row r="13" spans="2:6" ht="14">
       <c r="B13" s="25" t="s">
@@ -3188,11 +3188,11 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="135" t="str">
+      <c r="E13" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Sandrae Simpson</v>
       </c>
-      <c r="F13" s="136"/>
+      <c r="F13" s="135"/>
     </row>
     <row r="14" spans="2:6" ht="14">
       <c r="B14" s="25" t="s">
@@ -3201,11 +3201,11 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="135" t="str">
+      <c r="E14" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Randy Sindole</v>
       </c>
-      <c r="F14" s="136"/>
+      <c r="F14" s="135"/>
     </row>
     <row r="15" spans="2:6" ht="14">
       <c r="B15" s="25" t="s">
@@ -3214,11 +3214,11 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="135" t="str">
+      <c r="E15" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Ellen Smith</v>
       </c>
-      <c r="F15" s="136"/>
+      <c r="F15" s="135"/>
     </row>
     <row r="16" spans="2:6" ht="14">
       <c r="B16" s="25" t="s">
@@ -3227,11 +3227,11 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="135" t="str">
+      <c r="E16" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Tuome Vuanuo</v>
       </c>
-      <c r="F16" s="136"/>
+      <c r="F16" s="135"/>
     </row>
     <row r="17" spans="2:6" ht="14">
       <c r="B17" s="25" t="s">
@@ -3240,11 +3240,11 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="135" t="str">
+      <c r="E17" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Tadeuz Szcznyck</v>
       </c>
-      <c r="F17" s="136"/>
+      <c r="F17" s="135"/>
     </row>
     <row r="18" spans="2:6" ht="14">
       <c r="B18" s="25" t="s">
@@ -3253,21 +3253,14 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="135" t="str">
+      <c r="E18" s="134" t="str">
         <f>_xlfn.CONCAT(C18, " ", B18)</f>
         <v>Tammy Wu</v>
       </c>
-      <c r="F18" s="136"/>
+      <c r="F18" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3278,6 +3271,13 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3867,8 +3867,8 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -4132,8 +4132,8 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="B2:C14"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -4185,43 +4185,58 @@
       <c r="B8" s="75">
         <v>7.2499999999999995E-2</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="12">
+        <f t="dataTable" ref="C8:C14" dt2D="0" dtr="0" r1="C3"/>
+        <v>1590.1751010137643</v>
+      </c>
     </row>
     <row r="9" spans="2:3" ht="16">
       <c r="B9" s="75">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="12">
+        <v>1625.7805911544106</v>
+      </c>
     </row>
     <row r="10" spans="2:3" ht="16">
       <c r="B10" s="75">
         <v>7.7499999999999999E-2</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="12">
+        <v>1661.7232770342728</v>
+      </c>
     </row>
     <row r="11" spans="2:3" ht="16">
       <c r="B11" s="75">
         <v>8.2500000000000004E-2</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="12">
+        <v>1734.5902963096128</v>
+      </c>
     </row>
     <row r="12" spans="2:3" ht="16">
       <c r="B12" s="75">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="12">
+        <v>1771.4995836166886</v>
+      </c>
     </row>
     <row r="13" spans="2:3" ht="16">
       <c r="B13" s="75">
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="12">
+        <v>1808.7159994580018</v>
+      </c>
     </row>
     <row r="14" spans="2:3" ht="16">
       <c r="B14" s="75">
         <v>0.09</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="12">
+        <v>1846.2319999966555</v>
+      </c>
     </row>
   </sheetData>
   <printOptions gridLines="1" gridLinesSet="0"/>

</xml_diff>

<commit_message>
Creating Scenarios in Excel
</commit_message>
<xml_diff>
--- a/Section 29: Mastering Excel's "What If?" Tools/Resources/Excel103-AdvancedExercises.xlsx
+++ b/Section 29: Mastering Excel's "What If?" Tools/Resources/Excel103-AdvancedExercises.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolinecrandell/Documents/Employment/*Applications/2022.12 Job Apps/GitHub/excel/Section 29: Mastering Excel's &quot;What If?&quot; Tools/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548E3918-08AE-FA4C-AC94-FFE5248D8570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A94DE6F-39EF-B541-AC8D-CFEEE753EE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16680" firstSheet="7" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16680" firstSheet="8" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -1972,13 +1972,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3046,10 +3046,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="136" t="s">
+      <c r="E2" s="134" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="136"/>
+      <c r="F2" s="134"/>
     </row>
     <row r="3" spans="2:6" ht="14">
       <c r="B3" s="25" t="s">
@@ -3058,11 +3058,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="134" t="str">
+      <c r="E3" s="135" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="135"/>
+      <c r="F3" s="136"/>
     </row>
     <row r="4" spans="2:6" ht="14">
       <c r="B4" s="25" t="s">
@@ -3071,11 +3071,11 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="134" t="str">
+      <c r="E4" s="135" t="str">
         <f>_xlfn.CONCAT(C4, " ", B4)</f>
         <v>Joe Gonzales</v>
       </c>
-      <c r="F4" s="135"/>
+      <c r="F4" s="136"/>
     </row>
     <row r="5" spans="2:6" ht="14">
       <c r="B5" s="25" t="s">
@@ -3084,11 +3084,11 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="134" t="str">
+      <c r="E5" s="135" t="str">
         <f t="shared" ref="E5:E17" si="0">_xlfn.CONCAT(C5, " ", B5)</f>
         <v>Gail Scote</v>
       </c>
-      <c r="F5" s="135"/>
+      <c r="F5" s="136"/>
     </row>
     <row r="6" spans="2:6" ht="14">
       <c r="B6" s="25" t="s">
@@ -3097,11 +3097,11 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="134" t="str">
+      <c r="E6" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Sheryl Kane</v>
       </c>
-      <c r="F6" s="135"/>
+      <c r="F6" s="136"/>
     </row>
     <row r="7" spans="2:6" ht="14">
       <c r="B7" s="25" t="s">
@@ -3110,11 +3110,11 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="134" t="str">
+      <c r="E7" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Kendrick Hapsbuch</v>
       </c>
-      <c r="F7" s="135"/>
+      <c r="F7" s="136"/>
     </row>
     <row r="8" spans="2:6" ht="14">
       <c r="B8" s="25" t="s">
@@ -3123,11 +3123,11 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="134" t="str">
+      <c r="E8" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Mark Henders</v>
       </c>
-      <c r="F8" s="135"/>
+      <c r="F8" s="136"/>
     </row>
     <row r="9" spans="2:6" ht="14">
       <c r="B9" s="25" t="s">
@@ -3136,11 +3136,11 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="134" t="str">
+      <c r="E9" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Katie Atherton</v>
       </c>
-      <c r="F9" s="135"/>
+      <c r="F9" s="136"/>
     </row>
     <row r="10" spans="2:6" ht="14">
       <c r="B10" s="25" t="s">
@@ -3149,11 +3149,11 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="134" t="str">
+      <c r="E10" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Frank Bellwood</v>
       </c>
-      <c r="F10" s="135"/>
+      <c r="F10" s="136"/>
     </row>
     <row r="11" spans="2:6" ht="14">
       <c r="B11" s="25" t="s">
@@ -3162,11 +3162,11 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="134" t="str">
+      <c r="E11" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Linda Cooper</v>
       </c>
-      <c r="F11" s="135"/>
+      <c r="F11" s="136"/>
     </row>
     <row r="12" spans="2:6" ht="14">
       <c r="B12" s="25" t="s">
@@ -3175,11 +3175,11 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="134" t="str">
+      <c r="E12" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Brent Cronwith</v>
       </c>
-      <c r="F12" s="135"/>
+      <c r="F12" s="136"/>
     </row>
     <row r="13" spans="2:6" ht="14">
       <c r="B13" s="25" t="s">
@@ -3188,11 +3188,11 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="134" t="str">
+      <c r="E13" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Sandrae Simpson</v>
       </c>
-      <c r="F13" s="135"/>
+      <c r="F13" s="136"/>
     </row>
     <row r="14" spans="2:6" ht="14">
       <c r="B14" s="25" t="s">
@@ -3201,11 +3201,11 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="134" t="str">
+      <c r="E14" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Randy Sindole</v>
       </c>
-      <c r="F14" s="135"/>
+      <c r="F14" s="136"/>
     </row>
     <row r="15" spans="2:6" ht="14">
       <c r="B15" s="25" t="s">
@@ -3214,11 +3214,11 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="134" t="str">
+      <c r="E15" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Ellen Smith</v>
       </c>
-      <c r="F15" s="135"/>
+      <c r="F15" s="136"/>
     </row>
     <row r="16" spans="2:6" ht="14">
       <c r="B16" s="25" t="s">
@@ -3227,11 +3227,11 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="134" t="str">
+      <c r="E16" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Tuome Vuanuo</v>
       </c>
-      <c r="F16" s="135"/>
+      <c r="F16" s="136"/>
     </row>
     <row r="17" spans="2:6" ht="14">
       <c r="B17" s="25" t="s">
@@ -3240,11 +3240,11 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="134" t="str">
+      <c r="E17" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Tadeuz Szcznyck</v>
       </c>
-      <c r="F17" s="135"/>
+      <c r="F17" s="136"/>
     </row>
     <row r="18" spans="2:6" ht="14">
       <c r="B18" s="25" t="s">
@@ -3253,14 +3253,21 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="134" t="str">
+      <c r="E18" s="135" t="str">
         <f>_xlfn.CONCAT(C18, " ", B18)</f>
         <v>Tammy Wu</v>
       </c>
-      <c r="F18" s="135"/>
+      <c r="F18" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3271,13 +3278,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4132,7 +4132,7 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="B2:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -4254,8 +4254,8 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="B2:G14"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C14"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -4296,19 +4296,19 @@
       </c>
       <c r="D3" s="113">
         <f>C3*C11+C3</f>
-        <v>88106.894249999998</v>
+        <v>86145.172500000001</v>
       </c>
       <c r="E3" s="113">
         <f>D3*C11+D3</f>
-        <v>91014.421760249999</v>
+        <v>87006.624225000007</v>
       </c>
       <c r="F3" s="113">
         <f>E3*C11+E3</f>
-        <v>94017.897678338253</v>
+        <v>87876.69046725001</v>
       </c>
       <c r="G3" s="113">
         <f>SUM(C3:F3)</f>
-        <v>358431.46368858824</v>
+        <v>346320.73719224997</v>
       </c>
     </row>
     <row r="4" spans="2:7">
@@ -4320,19 +4320,19 @@
       </c>
       <c r="D4" s="113">
         <f>C4*C12+C4</f>
-        <v>77636.748749999999</v>
+        <v>76650.162500000006</v>
       </c>
       <c r="E4" s="113">
         <f>D4*C12+D4</f>
-        <v>79422.39397125</v>
+        <v>77416.66412500001</v>
       </c>
       <c r="F4" s="113">
         <f>E4*C12+E4</f>
-        <v>81249.109032588749</v>
+        <v>78190.830766250016</v>
       </c>
       <c r="G4" s="113">
         <f>SUM(C4:F4)</f>
-        <v>314199.50175383873</v>
+        <v>308148.90739125002</v>
       </c>
     </row>
     <row r="5" spans="2:7">
@@ -4344,19 +4344,19 @@
       </c>
       <c r="D5" s="113">
         <f>C5*C13+C5</f>
-        <v>94462.778619999997</v>
+        <v>91474.023399999991</v>
       </c>
       <c r="E5" s="113">
         <f>D5*C13+D5</f>
-        <v>98524.678100659992</v>
+        <v>92388.763633999988</v>
       </c>
       <c r="F5" s="113">
         <f>E5*C13+E5</f>
-        <v>102761.23925898837</v>
+        <v>93312.651270339993</v>
       </c>
       <c r="G5" s="113">
         <f>SUM(C5:F5)</f>
-        <v>386317.03597964835</v>
+        <v>367743.77830433997</v>
       </c>
     </row>
     <row r="6" spans="2:7">
@@ -4368,19 +4368,19 @@
       </c>
       <c r="D6" s="113">
         <f>C6*C14+C6</f>
-        <v>66622.119749999998</v>
+        <v>66556.222500000003</v>
       </c>
       <c r="E6" s="113">
         <f>D6*C14+D6</f>
-        <v>67354.963067249992</v>
+        <v>67221.784725000005</v>
       </c>
       <c r="F6" s="113">
         <f>E6*C14+E6</f>
-        <v>68095.867660989737</v>
+        <v>67894.00257225</v>
       </c>
       <c r="G6" s="113">
         <f>SUM(C6:F6)</f>
-        <v>267970.20047823974</v>
+        <v>267569.25979725004</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="16">
@@ -4393,19 +4393,19 @@
       </c>
       <c r="D7" s="77">
         <f>SUM(D3:D6)</f>
-        <v>326828.54136999999</v>
+        <v>320825.58090000006</v>
       </c>
       <c r="E7" s="77">
         <f>SUM(E3:E6)</f>
-        <v>336316.45689940994</v>
+        <v>324033.83670900005</v>
       </c>
       <c r="F7" s="77">
         <f>SUM(F3:F6)</f>
-        <v>346124.11363090511</v>
+        <v>327274.17507609003</v>
       </c>
       <c r="G7" s="77">
         <f>SUM(G3:G6)</f>
-        <v>1326918.201900315</v>
+        <v>1289782.68268509</v>
       </c>
     </row>
     <row r="10" spans="2:7">
@@ -4419,7 +4419,7 @@
         <v>258</v>
       </c>
       <c r="C11" s="115">
-        <v>3.3000000000000002E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="12" spans="2:7">
@@ -4427,7 +4427,7 @@
         <v>257</v>
       </c>
       <c r="C12" s="115">
-        <v>2.3E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="13" spans="2:7">
@@ -4435,7 +4435,7 @@
         <v>256</v>
       </c>
       <c r="C13" s="115">
-        <v>4.2999999999999997E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="14" spans="2:7">
@@ -4443,10 +4443,30 @@
         <v>255</v>
       </c>
       <c r="C14" s="115">
-        <v>1.0999999999999999E-2</v>
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>
+  <scenarios current="2" show="2">
+    <scenario name="Default Scenario" locked="1" count="4" user="Crandell, Caroline" comment="Created by Crandell, Caroline on 11/25/2023">
+      <inputCells r="C11" val="0.033" numFmtId="10"/>
+      <inputCells r="C12" val="0.023" numFmtId="10"/>
+      <inputCells r="C13" val="0.043" numFmtId="10"/>
+      <inputCells r="C14" val="0.011" numFmtId="10"/>
+    </scenario>
+    <scenario name="Best Case Scenario" locked="1" count="4" user="Crandell, Caroline" comment="Created by Crandell, Caroline on 11/25/2023">
+      <inputCells r="C11" val="0.05" numFmtId="10"/>
+      <inputCells r="C12" val="0.08" numFmtId="10"/>
+      <inputCells r="C13" val="0.065" numFmtId="10"/>
+      <inputCells r="C14" val="0.03" numFmtId="10"/>
+    </scenario>
+    <scenario name="Worst Case Scenario" locked="1" count="4" user="Crandell, Caroline" comment="Created by Crandell, Caroline on 11/25/2023">
+      <inputCells r="C11" val="0.01" numFmtId="10"/>
+      <inputCells r="C12" val="0.01" numFmtId="10"/>
+      <inputCells r="C13" val="0.01" numFmtId="10"/>
+      <inputCells r="C14" val="0.01" numFmtId="10"/>
+    </scenario>
+  </scenarios>
   <mergeCells count="1">
     <mergeCell ref="B10:C10"/>
   </mergeCells>

</xml_diff>